<commit_message>
Data now shows file name
</commit_message>
<xml_diff>
--- a/DataPSNR.xlsx
+++ b/DataPSNR.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,10 +436,15 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>File Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>PSNR</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>MSE</t>
         </is>
@@ -449,10 +454,15 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>CrowGSM.jpg</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>32.7767420813213</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>34.30884933430299</v>
       </c>
     </row>
@@ -460,10 +470,15 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>GSM_TE.jpg</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>30.35833153696467</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>59.87523172072117</v>
       </c>
     </row>

</xml_diff>